<commit_message>
Documentation Updated for 2nd semester. Removing Usability Study and server risk.
</commit_message>
<xml_diff>
--- a/Management/Risk Table.xlsx
+++ b/Management/Risk Table.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Desktop\Classes\Senior Project\Repo\Management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" tabRatio="289"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sp1" sheetId="1" r:id="rId2"/>
     <sheet name="Orig" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>NOAA permenantly goes offline</t>
   </si>
@@ -376,6 +381,157 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -392,20 +548,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
@@ -451,37 +593,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <strike val="0"/>
@@ -498,6 +609,9 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -509,116 +623,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -626,36 +631,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:G10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:G10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:G8" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:G8"/>
   <sortState ref="A2:F12">
     <sortCondition descending="1" ref="D1:D12"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="7" name="No." dataDxfId="17"/>
-    <tableColumn id="1" name="Risk" dataDxfId="13"/>
-    <tableColumn id="2" name="Likelihood" dataDxfId="12"/>
-    <tableColumn id="3" name="Impact" dataDxfId="11"/>
-    <tableColumn id="4" name="Score" dataDxfId="9">
-      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="10"/>
-    <tableColumn id="6" name="Contingency Plan" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:G11"/>
-  <sortState ref="A2:G11">
-    <sortCondition descending="1" ref="E1:E11"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="No." dataDxfId="24"/>
@@ -667,6 +654,27 @@
     </tableColumn>
     <tableColumn id="5" name="Mitigation Strategy" dataDxfId="19"/>
     <tableColumn id="6" name="Contingency Plan" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:G11"/>
+  <sortState ref="A2:G11">
+    <sortCondition descending="1" ref="E1:E11"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="No." dataDxfId="15"/>
+    <tableColumn id="1" name="Risk" dataDxfId="14"/>
+    <tableColumn id="2" name="Likelihood" dataDxfId="13"/>
+    <tableColumn id="3" name="Impact" dataDxfId="12"/>
+    <tableColumn id="4" name="Score" dataDxfId="11">
+      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="10"/>
+    <tableColumn id="6" name="Contingency Plan" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,7 +744,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -771,7 +779,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -980,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1042,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="13">
-        <f t="shared" ref="E2:E10" si="0">PRODUCT(C2,D2)</f>
+        <f t="shared" ref="E2:E8" si="0">PRODUCT(C2,D2)</f>
         <v>100</v>
       </c>
       <c r="F2" s="17" t="s">
@@ -1044,201 +1052,153 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C3" s="12">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>6</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12">
         <v>5</v>
       </c>
-      <c r="D3" s="12">
-        <v>7</v>
-      </c>
-      <c r="E3" s="13">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="D4" s="12">
         <v>4</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="12">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12">
-        <v>8</v>
-      </c>
       <c r="E4" s="13">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="12">
-        <v>5</v>
-      </c>
-      <c r="D5" s="12">
-        <v>4</v>
-      </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="56.25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C6" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" s="12">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="12">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
       </c>
       <c r="D8" s="12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>10</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12">
-        <v>10</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
         <v>11</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12">
-        <v>8</v>
-      </c>
-      <c r="E10" s="13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E10">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="E1:E8">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="50"/>
@@ -1248,7 +1208,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="50"/>
@@ -1258,7 +1218,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1339,7 +1299,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="10">
-        <f>PRODUCT(C2,D2)</f>
+        <f t="shared" ref="E2:E11" si="0">PRODUCT(C2,D2)</f>
         <v>100</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -1364,7 +1324,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="10">
-        <f>PRODUCT(C3,D3)</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1389,7 +1349,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="10">
-        <f>PRODUCT(C4,D4)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -1414,7 +1374,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="10">
-        <f>PRODUCT(C5,D5)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -1439,7 +1399,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="10">
-        <f>PRODUCT(C6,D6)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -1464,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="10">
-        <f>PRODUCT(C7,D7)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -1489,7 +1449,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="10">
-        <f>PRODUCT(C8,D8)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1514,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="10">
-        <f>PRODUCT(C9,D9)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -1539,7 +1499,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="10">
-        <f>PRODUCT(C10,D10)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -1565,7 +1525,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="10">
-        <f>PRODUCT(C11,D11)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -1860,7 +1820,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="10">
-        <f>PRODUCT(C2,D2)</f>
+        <f t="shared" ref="E2:E12" si="0">PRODUCT(C2,D2)</f>
         <v>100</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -1884,7 +1844,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="10">
-        <f>PRODUCT(C3,D3)</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1908,7 +1868,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="10">
-        <f>PRODUCT(C4,D4)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -1932,7 +1892,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="10">
-        <f>PRODUCT(C5,D5)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -1956,7 +1916,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="10">
-        <f>PRODUCT(C6,D6)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -1980,7 +1940,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="10">
-        <f>PRODUCT(C7,D7)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -2004,7 +1964,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="10">
-        <f>PRODUCT(C8,D8)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -2028,7 +1988,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="10">
-        <f>PRODUCT(C9,D9)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -2052,7 +2012,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="10">
-        <f>PRODUCT(C10,D10)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -2076,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="10">
-        <f>PRODUCT(C11,D11)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -2100,7 +2060,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="10">
-        <f>PRODUCT(C12,D12)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F12" s="9" t="s">

</xml_diff>

<commit_message>
Fixed Risk table format, and Finished status report 2
</commit_message>
<xml_diff>
--- a/Management/Risk Table.xlsx
+++ b/Management/Risk Table.xlsx
@@ -12,16 +12,20 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" tabRatio="289"/>
   </bookViews>
   <sheets>
-    <sheet name="Sp2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sp1" sheetId="1" r:id="rId2"/>
-    <sheet name="Orig" sheetId="3" r:id="rId3"/>
+    <sheet name="Sp3" sheetId="4" r:id="rId1"/>
+    <sheet name="Sp2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sp1" sheetId="1" r:id="rId3"/>
+    <sheet name="Orig" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="37">
   <si>
     <t>NOAA permenantly goes offline</t>
   </si>
@@ -138,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +185,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -251,11 +261,162 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -626,7 +787,12 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -639,52 +805,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:G8" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A1:G8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G8"/>
   <sortState ref="A2:F12">
     <sortCondition descending="1" ref="D1:D12"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="7" name="No." dataDxfId="24"/>
-    <tableColumn id="1" name="Risk" dataDxfId="23"/>
-    <tableColumn id="2" name="Likelihood" dataDxfId="22"/>
-    <tableColumn id="3" name="Impact" dataDxfId="21"/>
-    <tableColumn id="4" name="Score" dataDxfId="20">
-      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="19"/>
-    <tableColumn id="6" name="Contingency Plan" dataDxfId="18"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:G11"/>
-  <sortState ref="A2:G11">
-    <sortCondition descending="1" ref="E1:E11"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="7" name="No." dataDxfId="15"/>
-    <tableColumn id="1" name="Risk" dataDxfId="14"/>
-    <tableColumn id="2" name="Likelihood" dataDxfId="13"/>
-    <tableColumn id="3" name="Impact" dataDxfId="12"/>
-    <tableColumn id="4" name="Score" dataDxfId="11">
-      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="10"/>
-    <tableColumn id="6" name="Contingency Plan" dataDxfId="9"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:G12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G12"/>
-  <sortState ref="A2:G12">
-    <sortCondition descending="1" ref="E1:E12"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="No." dataDxfId="6"/>
@@ -696,6 +820,69 @@
     </tableColumn>
     <tableColumn id="5" name="Mitigation Strategy" dataDxfId="1"/>
     <tableColumn id="6" name="Contingency Plan" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:G10" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A1:G10"/>
+  <sortState ref="A2:F12">
+    <sortCondition descending="1" ref="D1:D12"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="No." dataDxfId="35"/>
+    <tableColumn id="1" name="Risk" dataDxfId="34"/>
+    <tableColumn id="2" name="Likelihood" dataDxfId="33"/>
+    <tableColumn id="3" name="Impact" dataDxfId="32"/>
+    <tableColumn id="4" name="Score" dataDxfId="31">
+      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="30"/>
+    <tableColumn id="6" name="Contingency Plan" dataDxfId="29"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:G11"/>
+  <sortState ref="A2:G11">
+    <sortCondition descending="1" ref="E1:E11"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="No." dataDxfId="26"/>
+    <tableColumn id="1" name="Risk" dataDxfId="25"/>
+    <tableColumn id="2" name="Likelihood" dataDxfId="24"/>
+    <tableColumn id="3" name="Impact" dataDxfId="23"/>
+    <tableColumn id="4" name="Score" dataDxfId="22">
+      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="21"/>
+    <tableColumn id="6" name="Contingency Plan" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:G12"/>
+  <sortState ref="A2:G12">
+    <sortCondition descending="1" ref="E1:E12"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="No." dataDxfId="17"/>
+    <tableColumn id="1" name="Risk" dataDxfId="16"/>
+    <tableColumn id="2" name="Likelihood" dataDxfId="15"/>
+    <tableColumn id="3" name="Impact" dataDxfId="14"/>
+    <tableColumn id="4" name="Score" dataDxfId="13">
+      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="12"/>
+    <tableColumn id="6" name="Contingency Plan" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -991,7 +1178,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1385,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E8">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="50"/>
@@ -1208,7 +1395,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="50"/>
@@ -1218,7 +1405,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1238,10 +1425,299 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="11">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10">
+        <v>100</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="11">
+        <v>5</v>
+      </c>
+      <c r="D3" s="11">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10">
+        <v>35</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="11">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10">
+        <v>32</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="11">
+        <v>5</v>
+      </c>
+      <c r="D5" s="11">
+        <v>4</v>
+      </c>
+      <c r="E5" s="10">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="11">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="10">
+        <v>16</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>10</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>10</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19">
+        <v>10</v>
+      </c>
+      <c r="E9" s="13">
+        <v>10</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>11</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19">
+        <v>8</v>
+      </c>
+      <c r="E10" s="13">
+        <v>8</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1768,7 +2244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>

</xml_diff>